<commit_message>
udpated new users and db structure excel
</commit_message>
<xml_diff>
--- a/project_notes/database-structure.xlsx
+++ b/project_notes/database-structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16020" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Spouse" sheetId="3" r:id="rId3"/>
     <sheet name="Car" sheetId="4" r:id="rId4"/>
     <sheet name="Kids" sheetId="5" r:id="rId5"/>
-    <sheet name="gamelog" sheetId="6" r:id="rId6"/>
+    <sheet name="Gamelog" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>first_name</t>
   </si>
@@ -86,24 +86,9 @@
     <t>username</t>
   </si>
   <si>
-    <t>house_id</t>
-  </si>
-  <si>
-    <t>spouse_id</t>
-  </si>
-  <si>
-    <t>car_id</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
-    <t>created_date</t>
-  </si>
-  <si>
-    <t>updated_date</t>
-  </si>
-  <si>
     <t>make</t>
   </si>
   <si>
@@ -114,6 +99,12 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>spouse</t>
+  </si>
+  <si>
+    <t>car</t>
   </si>
 </sst>
 </file>
@@ -594,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -720,7 +711,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -730,13 +721,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>7</v>
@@ -771,7 +762,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -804,10 +795,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -816,27 +807,21 @@
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>